<commit_message>
Change variable of data
</commit_message>
<xml_diff>
--- a/normal-multivariate-distribution-using-r.xlsx
+++ b/normal-multivariate-distribution-using-r.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Datasudo\9. Statistika Multivariate Terapan\Bahan\Praktikum\Modul 2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="14355" windowHeight="6465"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -17,51 +22,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="150">
   <si>
-    <t>Tahun/Bulan</t>
-  </si>
-  <si>
-    <t>Kesehatan</t>
-  </si>
-  <si>
-    <t>Desember</t>
-  </si>
-  <si>
     <t>November</t>
   </si>
   <si>
-    <t>Oktober</t>
-  </si>
-  <si>
     <t>September</t>
   </si>
   <si>
-    <t>Agustus</t>
-  </si>
-  <si>
-    <t>Juli</t>
-  </si>
-  <si>
-    <t>Juni</t>
-  </si>
-  <si>
-    <t>Mei</t>
-  </si>
-  <si>
     <t>April</t>
   </si>
   <si>
-    <t>Maret</t>
-  </si>
-  <si>
-    <t>Februari</t>
-  </si>
-  <si>
-    <t>Januari</t>
-  </si>
-  <si>
-    <t>Inflasi Indonesia Menurut Kelompok Pengeluaran Tahun 2006-2016</t>
-  </si>
-  <si>
     <t>0.45</t>
   </si>
   <si>
@@ -458,13 +427,49 @@
     <t>1.06</t>
   </si>
   <si>
-    <t>Makanan Jadi, Minuman, Rokok, dan Tembakau</t>
-  </si>
-  <si>
-    <t>Perumahan, Air, Listrik, Gas, dan Bahan Bakar</t>
-  </si>
-  <si>
-    <t>Pendidikan, Rekreasi, dan Olahraga</t>
+    <t>Month/Year</t>
+  </si>
+  <si>
+    <t>Indonesia Inflation by Expenditure Group Year 2006-2016</t>
+  </si>
+  <si>
+    <t>Food, Drinks, Cigarettes, and Tobacco</t>
+  </si>
+  <si>
+    <t>Housing, Water, Electricity, Gas, and Fuel</t>
+  </si>
+  <si>
+    <t>Healt</t>
+  </si>
+  <si>
+    <t>Education, Recreation, and Sports</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>January</t>
   </si>
 </sst>
 </file>
@@ -1439,6 +1444,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1455,8 +1463,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>361949</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1466,7 +1474,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5714999" y="438149"/>
-          <a:ext cx="4772025" cy="2352676"/>
+          <a:ext cx="4772025" cy="2219326"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1493,327 +1501,87 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="id-ID" sz="1100" b="1"/>
-            <a:t>SOAL</a:t>
+            <a:t>QUESTION</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l"/>
+          <a:pPr algn="just"/>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>1. Lakukan pengujian data </a:t>
+            <a:rPr lang="id-ID" sz="1100" b="0"/>
+            <a:t>1. Do a missing data test against the following inflation data and then overcome</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100" i="1">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>missing</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> terhadap data inflasi</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
+            <a:rPr lang="en-US" sz="1100" b="0"/>
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>berikut kemudian atasi</a:t>
-          </a:r>
-          <a:endParaRPr lang="id-ID" sz="1100" baseline="0">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>     data </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" i="1" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>missing</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> tersebut dengan cara</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> :</a:t>
+            <a:rPr lang="id-ID" sz="1100" b="0"/>
+            <a:t>Data missing by way of:</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l"/>
+          <a:pPr algn="just"/>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>     a. menghapus data </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" i="1" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>missing</a:t>
+            <a:rPr lang="id-ID" sz="1100" b="0"/>
+            <a:t>      A. Delete missing data</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l"/>
+          <a:pPr algn="just"/>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>     b. tanpa menghapus data </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" i="1" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>missing</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> (lakukan estimasi terhadap data </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" i="1" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>missing)</a:t>
+            <a:rPr lang="id-ID" sz="1100" b="0"/>
+            <a:t>      B. Without deleting missing data (do estimation of missing data)</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l"/>
+          <a:pPr algn="just"/>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>2.  Lakukan pengujian terhadap data </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" i="1" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>outlier! </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Jika terdapat data </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" i="1" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>outlier,</a:t>
+            <a:rPr lang="id-ID" sz="1100" b="0"/>
+            <a:t>2. Test outlier data! If there are outlier data,</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l"/>
+          <a:pPr algn="just"/>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>      pertimbangkan apakah anda akan mempertahankan data </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" i="1" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>outlier </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>tersebut</a:t>
+            <a:rPr lang="id-ID" sz="1100" b="0"/>
+            <a:t>       Consider whether you will retain the outlier data</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l"/>
+          <a:pPr algn="just"/>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>      atau membuang data </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" i="1" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>outlier, </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>jelaskan alasan anda !</a:t>
+            <a:rPr lang="id-ID" sz="1100" b="0"/>
+            <a:t>       Or remove outlier data, explain your reasons!</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l"/>
+          <a:pPr algn="just"/>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>3. Lakukan pengujian Normalitas Multivariat terhadap data inflasi </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1" u="sng" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>secara</a:t>
+            <a:rPr lang="id-ID" sz="1100" b="0"/>
+            <a:t>3. Perform Multivariate Normality testing of inflation data in a manner</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l"/>
+          <a:pPr algn="just"/>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1" u="none" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>     </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1" u="sng" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>keseluruhan</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>maupun untuk </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1" u="sng" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>masing-masing variabel </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>dengan :</a:t>
+            <a:rPr lang="id-ID" sz="1100" b="0"/>
+            <a:t>      Overall or for each variable with:</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l"/>
+          <a:pPr algn="just"/>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>     a. Metode grafis</a:t>
+            <a:rPr lang="id-ID" sz="1100" b="0"/>
+            <a:t>      A. Graphical method</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:pPr algn="l"/>
+          <a:pPr algn="just"/>
           <a:r>
-            <a:rPr lang="id-ID" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>     b. Uji hipotesis (minimal 2 metode yang berbeda) </a:t>
+            <a:rPr lang="id-ID" sz="1100" b="0"/>
+            <a:t>      B. Test the hypothesis (at least 2 different methods)</a:t>
           </a:r>
-          <a:endParaRPr lang="id-ID" sz="1100">
+          <a:endParaRPr lang="id-ID" sz="1100" b="0">
             <a:solidFill>
               <a:sysClr val="windowText" lastClr="000000"/>
             </a:solidFill>
@@ -1869,7 +1637,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1904,7 +1672,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2116,7 +1884,7 @@
   <dimension ref="A1:M134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2131,7 +1899,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>136</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -2142,22 +1910,22 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="4" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1</v>
+        <v>139</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -2172,19 +1940,19 @@
         <v>2016</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -2196,19 +1964,19 @@
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -2220,19 +1988,19 @@
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2244,19 +2012,19 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -2268,19 +2036,19 @@
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2292,19 +2060,19 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2316,19 +2084,19 @@
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -2340,19 +2108,19 @@
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -2364,19 +2132,19 @@
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -2388,53 +2156,53 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2442,215 +2210,215 @@
         <v>2015</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2658,217 +2426,217 @@
         <v>2014</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C32" s="3">
         <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2876,217 +2644,217 @@
         <v>2013</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="F48" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="F49" s="3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="F50" s="3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -3094,217 +2862,217 @@
         <v>2012</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D61" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E61" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -3312,217 +3080,217 @@
         <v>2011</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E71" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -3530,215 +3298,215 @@
         <v>2010</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C85" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -3746,217 +3514,217 @@
         <v>2009</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C91" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D91" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D91" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="E91" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3964,215 +3732,215 @@
         <v>2008</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="E100" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F100" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E104" s="3"/>
       <c r="F104" s="3" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -4180,217 +3948,217 @@
         <v>2007</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C112" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F112" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -4398,217 +4166,217 @@
         <v>2006</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="C123" s="3" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2" t="s">
-        <v>4</v>
+        <v>142</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2" t="s">
-        <v>7</v>
+        <v>144</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C130" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D130" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2" t="s">
-        <v>11</v>
+        <v>147</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
       <c r="B134" s="2" t="s">
-        <v>13</v>
+        <v>149</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>